<commit_message>
OSIS-658 XLS injection manages new column + apply to existing test xls files
</commit_message>
<xml_diff>
--- a/assessments/tests/resources/incorrect_formula.xlsx
+++ b/assessments/tests/resources/incorrect_formula.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="37">
   <si>
     <t xml:space="preserve">2017-18 – LOSIS1211</t>
   </si>
@@ -71,6 +71,9 @@
     <t xml:space="preserve">Prénom</t>
   </si>
   <si>
+    <t xml:space="preserve">Email</t>
+  </si>
+  <si>
     <t xml:space="preserve">Date de fin</t>
   </si>
   <si>
@@ -98,6 +101,9 @@
     <t xml:space="preserve">Adam</t>
   </si>
   <si>
+    <t xml:space="preserve">adam.smith@test.be</t>
+  </si>
+  <si>
     <t xml:space="preserve">-</t>
   </si>
   <si>
@@ -108,6 +114,9 @@
   </si>
   <si>
     <t xml:space="preserve">John</t>
+  </si>
+  <si>
+    <t xml:space="preserve">john.doe@test.be</t>
   </si>
   <si>
     <t xml:space="preserve">Etude</t>
@@ -132,7 +141,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="16">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -156,87 +165,6 @@
       <family val="0"/>
     </font>
     <font>
-      <b val="true"/>
-      <sz val="24"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="18"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF333333"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <i val="true"/>
-      <sz val="10"/>
-      <color rgb="FF808080"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF006600"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF996600"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFCC0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
@@ -244,7 +172,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -253,54 +181,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCCFFCC"/>
-        <bgColor rgb="FFCCFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCCCC"/>
-        <bgColor rgb="FFDDDDDD"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCC0000"/>
-        <bgColor rgb="FFFF0000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF000000"/>
-        <bgColor rgb="FF003300"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF808080"/>
-        <bgColor rgb="FF969696"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFDDDDDD"/>
-        <bgColor rgb="FFFFCCCC"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFC1C1C1"/>
-        <bgColor rgb="FFDDDDDD"/>
+        <bgColor rgb="FFCCCCFF"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -308,23 +194,8 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin">
-        <color rgb="FF808080"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF808080"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF808080"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF808080"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="36">
+  <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -348,92 +219,28 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="22">
+  <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Heading" xfId="20" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Heading 1" xfId="21" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Heading 2" xfId="22" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Text" xfId="23" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Note" xfId="24" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Footnote" xfId="25" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Status" xfId="26" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Good" xfId="27" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Neutral" xfId="28" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Bad" xfId="29" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Warning" xfId="30" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Error" xfId="31" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent" xfId="32" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 1" xfId="33" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 2" xfId="34" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 3" xfId="35" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -445,10 +252,10 @@
       <rgbColor rgb="FFFFFF00"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FFCC0000"/>
-      <rgbColor rgb="FF006600"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
       <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FF996600"/>
+      <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FFC1C1C1"/>
@@ -460,7 +267,7 @@
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
       <rgbColor rgb="FF0066CC"/>
-      <rgbColor rgb="FFDDDDDD"/>
+      <rgbColor rgb="FFCCCCFF"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FFFFFF00"/>
@@ -476,7 +283,7 @@
       <rgbColor rgb="FF99CCFF"/>
       <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCCCC"/>
+      <rgbColor rgb="FFFFCC99"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF99CC00"/>
@@ -503,13 +310,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K16"/>
+  <dimension ref="A1:L16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H14" activeCellId="0" sqref="H14"/>
+      <selection pane="topLeft" activeCell="H17" activeCellId="0" sqref="H17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.53"/>
@@ -517,33 +324,33 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="0" width="30"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="0" width="20"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="10.53"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="11" min="11" style="0" width="9.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="12" style="0" width="10.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="8" style="0" width="20"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="10.53"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="12" min="12" style="0" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="13" style="0" width="10.53"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
         <v>4</v>
       </c>
@@ -551,12 +358,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="0" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
         <v>7</v>
       </c>
@@ -564,7 +371,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
         <v>9</v>
       </c>
@@ -587,99 +394,112 @@
         <v>15</v>
       </c>
       <c r="H11" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="I11" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="I11" s="0" t="s">
+      <c r="J11" s="0" t="s">
         <v>4</v>
-      </c>
-      <c r="J11" s="0" t="s">
-        <v>16</v>
       </c>
       <c r="K11" s="0" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L11" s="0" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B12" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I12" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="L12" s="2" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="B13" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="C13" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="D13" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F12" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="H12" s="0" t="n">
-        <v>15</v>
-      </c>
-      <c r="J12" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="K12" s="2" t="n">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>21</v>
-      </c>
       <c r="E13" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="H13" s="0" t="e">
+        <v>30</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="I13" s="0" t="e">
         <f aca="false">ma(1,5,17)</f>
         <v>#NAME?</v>
       </c>
-      <c r="J13" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="K13" s="2" t="n">
+      <c r="K13" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="L13" s="2" t="n">
         <v>18</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K14" s="2" t="n">
+      <c r="L14" s="2" t="n">
         <v>17</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K15" s="2" t="n">
+      <c r="L15" s="2" t="n">
         <v>19</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K16" s="2" t="n">
+      <c r="L16" s="2" t="n">
         <v>20</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="H12" r:id="rId1" display="adam.smith@test.be"/>
+    <hyperlink ref="H13" r:id="rId2" display="john.doe@test.be"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -714,24 +534,24 @@
         <v>14</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>21</v>
       </c>
       <c r="D2" s="0" t="n">
         <v>14.7</v>
@@ -743,13 +563,13 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D3" s="0" t="n">
         <v>17.1</v>

</xml_diff>